<commit_message>
Finalização do script e início dos testes
</commit_message>
<xml_diff>
--- a/Teste Projeto NPS.xlsx
+++ b/Teste Projeto NPS.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6761D70C-5623-42FC-B33E-3C20FB869A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FELIPE.BICALETTO\Documents\npsZendesk\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ACCAF6-5B5B-4B3D-AB12-B43C40942D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
   <si>
     <t>Nome</t>
   </si>
@@ -45,7 +51,19 @@
     <t>Descrição</t>
   </si>
   <si>
-    <t>Tipo de cliente</t>
+    <t>Categoria do cliente</t>
+  </si>
+  <si>
+    <t>Tipo de usuário</t>
+  </si>
+  <si>
+    <t>Clínica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nota </t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
   <si>
     <t>Felipe Bicaletto</t>
@@ -60,14 +78,146 @@
     <t>Teste do projeto NPS</t>
   </si>
   <si>
+    <t>tipo_usuario_paciente</t>
+  </si>
+  <si>
+    <t>Comentário</t>
+  </si>
+  <si>
+    <t>Motivo de contato</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>user.name@gmail.com</t>
+  </si>
+  <si>
+    <t>Muito bom atendimento</t>
+  </si>
+  <si>
+    <t>Detrator</t>
+  </si>
+  <si>
+    <t>Péssimo atendimento</t>
+  </si>
+  <si>
+    <t>Atraso do Profissional</t>
+  </si>
+  <si>
+    <t>nps_etica_profissional</t>
+  </si>
+  <si>
+    <t>nps_corporate_mid_high</t>
+  </si>
+  <si>
+    <t>nps_lucas_guidi</t>
+  </si>
+  <si>
+    <t>Tags BU</t>
+  </si>
+  <si>
+    <t>nps_canais</t>
+  </si>
+  <si>
+    <t>nps_operadoras</t>
+  </si>
+  <si>
+    <t>nps_usabilidade_plataforma</t>
+  </si>
+  <si>
+    <t>nps_problemas_acesso_a_consulta</t>
+  </si>
+  <si>
+    <t>nps_atraso_profissional</t>
+  </si>
+  <si>
+    <t>tipo_usuario_gestor</t>
+  </si>
+  <si>
+    <t>tipo_usuario_profissional_de_saude</t>
+  </si>
+  <si>
+    <t>tipo_usuario_nao_identificado</t>
+  </si>
+  <si>
+    <t>Tags Motivos de contato</t>
+  </si>
+  <si>
+    <t>Tags Tipo de usuário</t>
+  </si>
+  <si>
+    <t>Tags CS</t>
+  </si>
+  <si>
+    <t>nps_thiago_kuchla</t>
+  </si>
+  <si>
+    <t>nps_milena_coelho</t>
+  </si>
+  <si>
+    <t>nps_lucas_braga</t>
+  </si>
+  <si>
+    <t>nps_raphael_gasparini</t>
+  </si>
+  <si>
+    <t>nps_bruna_loula</t>
+  </si>
+  <si>
+    <t>nps_camila_alves</t>
+  </si>
+  <si>
+    <t>nps_daniel_medeiros</t>
+  </si>
+  <si>
+    <t>nps_flavia_menezes</t>
+  </si>
+  <si>
+    <t>nps_guilherme_cristiano</t>
+  </si>
+  <si>
+    <t>nps_natalia_e_pedro</t>
+  </si>
+  <si>
+    <t>nps_pedro</t>
+  </si>
+  <si>
+    <t>nps_natalia_gomes</t>
+  </si>
+  <si>
+    <t>nps_carolina</t>
+  </si>
+  <si>
+    <t>100 - DASA - Interconsulta</t>
+  </si>
+  <si>
+    <t>195 - Hospital 9 de Julho</t>
+  </si>
+  <si>
+    <t>272 - Hospital Santa Paula</t>
+  </si>
+  <si>
     <t>Promotor</t>
+  </si>
+  <si>
+    <t>Neutro</t>
+  </si>
+  <si>
+    <t>nps_maíra_rodrigues</t>
+  </si>
+  <si>
+    <t>nps_sérgio_beserra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,25 +226,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF145F82"/>
+        <bgColor rgb="FF145F82"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF145F82"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -109,20 +288,140 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="15">
     <dxf>
       <font>
-        <color theme="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -138,14 +437,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B96925E3-8AA6-4045-8DAC-4D3865A4788A}" name="Tabela3" displayName="Tabela3" ref="A1:E2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:E2" xr:uid="{B96925E3-8AA6-4045-8DAC-4D3865A4788A}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C9F4EEA1-0053-400A-ABE6-C9BE0E7E3F42}" name="Nome"/>
-    <tableColumn id="2" xr3:uid="{5CA512F5-03EA-4AAE-9313-82CFF4AB993B}" name="E-mail"/>
-    <tableColumn id="3" xr3:uid="{BA4D16BF-8351-4F4B-964D-A5A06A4196C0}" name="Título"/>
-    <tableColumn id="4" xr3:uid="{B3AA16E5-3420-437B-8AE6-FD6237E3792F}" name="Descrição"/>
-    <tableColumn id="5" xr3:uid="{A1922F16-A061-4486-9EC1-4550E5913DB5}" name="Tipo de cliente"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B96925E3-8AA6-4045-8DAC-4D3865A4788A}" name="Tabela3" displayName="Tabela3" ref="A1:M4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:M4" xr:uid="{B96925E3-8AA6-4045-8DAC-4D3865A4788A}"/>
+  <tableColumns count="13">
+    <tableColumn id="1" xr3:uid="{C9F4EEA1-0053-400A-ABE6-C9BE0E7E3F42}" name="Nome" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{5CA512F5-03EA-4AAE-9313-82CFF4AB993B}" name="E-mail" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{BA4D16BF-8351-4F4B-964D-A5A06A4196C0}" name="Título" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{B3AA16E5-3420-437B-8AE6-FD6237E3792F}" name="Descrição" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A1922F16-A061-4486-9EC1-4550E5913DB5}" name="Categoria do cliente" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{D8EA5203-0129-4215-82CA-F1D4DDCA8C84}" name="Tipo de usuário" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{A7A77F0E-FD5E-48C4-8329-A2BCECF9CE33}" name="Clínica" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{28D42419-B01A-4C8E-9E96-A71C74FEAE39}" name="Nota " dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{EECDC656-9138-4DDD-B7DF-72FBF55D1BD4}" name="Login" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{BCBB97FE-C9E8-4B40-BB70-5FF67D39EB72}" name="Comentário" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{FEB35D72-04C0-4F63-BF36-D6569D7259EE}" name="Motivo de contato" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{1C3D3613-8B89-4A23-A5E0-F9A36D6045D6}" name="BU" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{7B924E0E-4A86-4C3F-89F8-0B1962140CCB}" name="CS" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -468,49 +775,186 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="7"/>
+    <col min="2" max="2" width="21.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="7"/>
+    <col min="4" max="4" width="22.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24.85546875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="7"/>
+    <col min="9" max="9" width="24" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="18.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="3">
+        <v>10</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" s="3">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="3">
+        <v>2</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -519,4 +963,152 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9A4C80-B31E-44D2-8662-4C59B4A8BF3B}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.5703125" customWidth="1"/>
+    <col min="2" max="2" width="35" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Projeto pronto para testes
</commit_message>
<xml_diff>
--- a/Teste Projeto NPS.xlsx
+++ b/Teste Projeto NPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FELIPE.BICALETTO\Documents\npsZendesk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ACCAF6-5B5B-4B3D-AB12-B43C40942D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA70A6B-5C24-43F1-98F1-BEE5C32A2FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Nome</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Péssimo atendimento</t>
-  </si>
-  <si>
-    <t>Atraso do Profissional</t>
   </si>
   <si>
     <t>nps_etica_profissional</t>
@@ -437,18 +434,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B96925E3-8AA6-4045-8DAC-4D3865A4788A}" name="Tabela3" displayName="Tabela3" ref="A1:M4" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B96925E3-8AA6-4045-8DAC-4D3865A4788A}" name="Tabela3" displayName="Tabela3" ref="A1:M4" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M4" xr:uid="{B96925E3-8AA6-4045-8DAC-4D3865A4788A}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{C9F4EEA1-0053-400A-ABE6-C9BE0E7E3F42}" name="Nome" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{5CA512F5-03EA-4AAE-9313-82CFF4AB993B}" name="E-mail" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{BA4D16BF-8351-4F4B-964D-A5A06A4196C0}" name="Título" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{B3AA16E5-3420-437B-8AE6-FD6237E3792F}" name="Descrição" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{A1922F16-A061-4486-9EC1-4550E5913DB5}" name="Categoria do cliente" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{D8EA5203-0129-4215-82CA-F1D4DDCA8C84}" name="Tipo de usuário" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{A7A77F0E-FD5E-48C4-8329-A2BCECF9CE33}" name="Clínica" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{28D42419-B01A-4C8E-9E96-A71C74FEAE39}" name="Nota " dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{EECDC656-9138-4DDD-B7DF-72FBF55D1BD4}" name="Login" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{C9F4EEA1-0053-400A-ABE6-C9BE0E7E3F42}" name="Nome" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{5CA512F5-03EA-4AAE-9313-82CFF4AB993B}" name="E-mail" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{BA4D16BF-8351-4F4B-964D-A5A06A4196C0}" name="Título" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B3AA16E5-3420-437B-8AE6-FD6237E3792F}" name="Descrição" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{A1922F16-A061-4486-9EC1-4550E5913DB5}" name="Categoria do cliente" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{D8EA5203-0129-4215-82CA-F1D4DDCA8C84}" name="Tipo de usuário" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{A7A77F0E-FD5E-48C4-8329-A2BCECF9CE33}" name="Clínica" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{28D42419-B01A-4C8E-9E96-A71C74FEAE39}" name="Nota " dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{EECDC656-9138-4DDD-B7DF-72FBF55D1BD4}" name="Login" dataDxfId="4"/>
     <tableColumn id="10" xr3:uid="{BCBB97FE-C9E8-4B40-BB70-5FF67D39EB72}" name="Comentário" dataDxfId="3"/>
     <tableColumn id="11" xr3:uid="{FEB35D72-04C0-4F63-BF36-D6569D7259EE}" name="Motivo de contato" dataDxfId="2"/>
     <tableColumn id="12" xr3:uid="{1C3D3613-8B89-4A23-A5E0-F9A36D6045D6}" name="BU" dataDxfId="1"/>
@@ -777,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,13 +847,13 @@
         <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H2" s="3">
         <v>10</v>
@@ -868,13 +865,13 @@
         <v>19</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -891,13 +888,13 @@
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H3" s="3">
         <v>5</v>
@@ -907,13 +904,13 @@
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -933,10 +930,10 @@
         <v>20</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H4" s="3">
         <v>2</v>
@@ -947,14 +944,14 @@
       <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>22</v>
+      <c r="K4" t="s">
+        <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -970,7 +967,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,30 +980,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,98 +1011,98 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>